<commit_message>
adding the  Product Minimum Facings Secondary to kpi list on KPI tab
</commit_message>
<xml_diff>
--- a/Projects/SANOFILB/Data/Template.xlsx
+++ b/Projects/SANOFILB/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -588,7 +588,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="88">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t xml:space="preserve">Secondary Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Minimum Facings Secondary</t>
   </si>
   <si>
     <t xml:space="preserve">MSL Compliance</t>
@@ -1073,7 +1076,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1124,6 +1127,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -1174,7 +1184,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1215,6 +1225,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1239,23 +1257,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1509,21 +1527,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1634,90 +1652,111 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="11" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="B8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="29.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="20" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1745,401 +1784,401 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="21" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="22" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="23" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="23" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="24" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="28" t="s">
         <v>33</v>
       </c>
+      <c r="H2" s="28" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="29" t="n">
+      <c r="A3" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="31" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="30" t="s">
+      <c r="D3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="31" t="n">
+      <c r="E3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="31" t="n">
+        <v>4048846012579</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="29" t="n">
-        <v>4048846012579</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="31" t="n">
+      <c r="F4" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="29" t="n">
+      <c r="A5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="31" t="n">
         <v>4048846008657</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="30" t="s">
+      <c r="D5" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="31" t="n">
+      <c r="E5" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="31" t="n">
+        <v>4048846006660</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="29" t="n">
-        <v>4048846006660</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="31" t="n">
+      <c r="F6" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="29" t="n">
+      <c r="A7" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="31" t="n">
         <v>3400936986046</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="31" t="n">
+      <c r="D7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="29" t="s">
+      <c r="A8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="31" t="n">
+      <c r="E8" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="30" t="s">
+      <c r="F9" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="31" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="31" t="n">
+      <c r="E10" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="29" t="n">
+      <c r="A11" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="31" t="n">
         <v>4048846008435</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="30" t="s">
+      <c r="D11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="31" t="n">
+      <c r="E11" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="31" t="n">
+        <v>3582910076018</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="29" t="n">
-        <v>3582910076018</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="31" t="n">
+      <c r="F12" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="29" t="n">
+      <c r="A13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="31" t="n">
         <v>5285003471926</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="31" t="n">
+      <c r="D13" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="32" t="s">
+      <c r="A14" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="31" t="n">
+        <v>5285003471933</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="29" t="n">
-        <v>5285003471933</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="31" t="n">
+      <c r="E14" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="B15" s="32"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2169,210 +2208,210 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="33" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="33" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="33" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="22" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="35" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="35" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="24" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="24"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="26"/>
       <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="35" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="36"/>
+      <c r="G2" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="A3" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="A4" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="A5" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="A6" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
+      <c r="A7" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="A8" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="A9" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="A10" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="A11" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
+      <c r="A12" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
+      <c r="A13" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
+      <c r="A14" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="A15" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="A16" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
+      <c r="A17" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
+      <c r="A18" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2396,315 +2435,315 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="41" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="41" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="41" width="26.4574898785425"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="41" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="41" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="42" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="43" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="37.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="43" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="43" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="44" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="26" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="G2" s="28" t="s">
         <v>33</v>
       </c>
+      <c r="H2" s="28" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="46" t="n">
+      <c r="E3" s="48" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="F3" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="47" t="n">
+      <c r="F3" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="49" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="48" t="n">
         <v>4048846012579</v>
       </c>
-      <c r="F4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="47" t="n">
+      <c r="F4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="48" t="n">
+        <v>5285003471933</v>
+      </c>
+      <c r="F6" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="47" t="n">
+      <c r="C7" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="48" t="n">
+        <v>3400936986046</v>
+      </c>
+      <c r="F8" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="49" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="46" t="n">
-        <v>5285003471933</v>
-      </c>
-      <c r="F6" s="47" t="n">
+      <c r="B9" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="47" t="n">
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
+      <c r="G10" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
+      <c r="B11" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="48" t="n">
+        <v>4048846008435</v>
+      </c>
+      <c r="F11" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="46" t="n">
-        <v>3400936986046</v>
-      </c>
-      <c r="F8" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="46" t="n">
-        <v>4048846008435</v>
-      </c>
-      <c r="F11" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="46" t="n">
+      <c r="E12" s="48" t="n">
         <v>3582910076018</v>
       </c>
-      <c r="F12" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="47" t="n">
+      <c r="F12" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="49" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2736,207 +2775,207 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="48" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="33" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="33" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="49" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="35" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="35" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="35" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="51" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="D2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="G2" s="53" t="s">
         <v>33</v>
       </c>
+      <c r="H2" s="53" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="54" t="s">
+      <c r="C3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="38" t="n">
+      <c r="E3" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="C4" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="38" t="n">
+      <c r="D4" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="38" t="n">
+      <c r="H4" s="40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="C5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="38" t="n">
+      <c r="D5" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="38" t="n">
+      <c r="H5" s="40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="C6" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="38" t="n">
+      <c r="D6" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="38" t="n">
+      <c r="H6" s="40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="B7" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="38" t="n">
+      <c r="C7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="C8" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="38" t="n">
+      <c r="D8" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2963,371 +3002,371 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="56" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="56" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="56" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="56" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="56" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="56" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="57" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="58" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="58" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="58" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="58" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="58" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="59" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="D2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="E2" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="F2" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="G2" s="53" t="s">
         <v>33</v>
       </c>
+      <c r="H2" s="53" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="59" t="n">
+      <c r="B3" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="61" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="D3" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="60" t="s">
+      <c r="D3" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="61" t="n">
+      <c r="E3" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="61" t="n">
+      <c r="G3" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="62"/>
+      <c r="H3" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="61" t="n">
+        <v>4048846012579</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="59" t="n">
-        <v>4048846012579</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="61" t="n">
+      <c r="F4" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="61" t="n">
+      <c r="G4" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="62"/>
+      <c r="H4" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="63" t="n">
+      <c r="B5" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="65" t="n">
         <v>4048846008657</v>
       </c>
-      <c r="D5" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="56" t="s">
+      <c r="D5" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="61" t="n">
+      <c r="E5" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="61" t="n">
+      <c r="G5" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="63" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="65" t="n">
+        <v>4048846006660</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="63" t="n">
-        <v>4048846006660</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="61" t="n">
+      <c r="F6" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="63" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="63" t="n">
+      <c r="B7" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="65" t="n">
         <v>3400936986046</v>
       </c>
-      <c r="D7" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="61" t="n">
+      <c r="D7" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="63" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="63" t="s">
+      <c r="B8" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="D8" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="61" t="n">
+      <c r="E8" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="61" t="n">
+      <c r="G8" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="61" t="n">
+      <c r="H8" s="63" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="56" t="s">
+      <c r="F9" s="63" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="63" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="61" t="n">
+      <c r="E10" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="65" t="n">
+        <v>4048846008435</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="61" t="n">
+      <c r="G11" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="52" t="s">
+      <c r="H11" s="63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="61" t="n">
+      <c r="B12" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="65" t="n">
+        <v>3582910076018</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="63" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="63" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" s="63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="65" t="n">
+        <v>5285003471926</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="63" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="52" t="s">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="63" t="n">
-        <v>4048846008435</v>
-      </c>
-      <c r="D11" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="G11" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="H11" s="61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="63" t="n">
-        <v>3582910076018</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" s="61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="63" t="n">
-        <v>5285003471926</v>
-      </c>
-      <c r="D13" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="61" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="65" t="n">
+        <v>5285003471933</v>
+      </c>
+      <c r="D14" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="63" t="n">
-        <v>5285003471933</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="61" t="n">
+      <c r="E14" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="61" t="n">
+      <c r="G14" s="63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="63" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>